<commit_message>
update orientation metric and include csv and plots
</commit_message>
<xml_diff>
--- a/Notebooks/2018August_Tomo27/UnbranchedFilamentOrientationInfo.xlsx
+++ b/Notebooks/2018August_Tomo27/UnbranchedFilamentOrientationInfo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Serwas_et_al_2021/PolarityAnalysis/CoordinatesAndPolarityInfoFiles/2018August_Tomo27/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/makamats/Google Drive/drubin_lab/Actin cortex project_local/polarity-analysis/Notebooks/2018August_Tomo27/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91DE52B7-FDFB-4B45-97E3-8D739A52838C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2170DC7-0687-9947-B614-5A9B34DF19D0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="41380" yWindow="980" windowWidth="27180" windowHeight="18080" xr2:uid="{4FFC31FB-4204-3046-BC24-842DC87851CE}"/>
   </bookViews>
@@ -26,7 +26,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -39,13 +38,13 @@
     <t>Average Difference</t>
   </si>
   <si>
-    <t>Contour no.</t>
-  </si>
-  <si>
     <t>Plus-end</t>
   </si>
   <si>
     <t>Minus-end</t>
+  </si>
+  <si>
+    <t>Contour Number In Model</t>
   </si>
 </sst>
 </file>
@@ -89,10 +88,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -409,9 +409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2391E6D-722D-C248-8E82-A2B7D756B3E7}">
   <dimension ref="A1:D83"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="C83" sqref="C83"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -421,14 +419,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>1</v>
+      <c r="A1" s="3" t="s">
+        <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>3</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>0</v>

</xml_diff>